<commit_message>
Some fixes TODO: -fix delete database if no database -fix license for OfficeOpenXml -fix null in ExcelManager -add transfer data from ExcelManager to SqlManager
</commit_message>
<xml_diff>
--- a/Office supplies acquisition table.xlsx
+++ b/Office supplies acquisition table.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walter\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Excel Reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F96A7EC8-7CB0-4F24-AADD-C2E015DE29A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5AAE71-8BBA-4797-81BC-1E1409E96138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6575F3AE-B7EC-453F-A456-52525722A30D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="1.2001" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -439,7 +439,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
BaseProjectDone TODO: Expand so any size excel sheet can be imported
</commit_message>
<xml_diff>
--- a/Office supplies acquisition table.xlsx
+++ b/Office supplies acquisition table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Excel Reader\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5AAE71-8BBA-4797-81BC-1E1409E96138}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5810735D-ED10-4465-822C-27255DB3CD40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6575F3AE-B7EC-453F-A456-52525722A30D}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{6575F3AE-B7EC-453F-A456-52525722A30D}"/>
   </bookViews>
   <sheets>
     <sheet name="1.2001" sheetId="1" r:id="rId1"/>
@@ -35,9 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
   <si>
-    <t>Order Date</t>
-  </si>
-  <si>
     <t>Region</t>
   </si>
   <si>
@@ -84,6 +81,9 @@
   </si>
   <si>
     <t>duck</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
   </si>
 </sst>
 </file>
@@ -439,7 +439,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,25 +449,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -475,13 +475,13 @@
         <v>36892</v>
       </c>
       <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -499,13 +499,13 @@
         <v>36893</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>32</v>
@@ -523,13 +523,13 @@
         <v>36894</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>54</v>
@@ -547,13 +547,13 @@
         <v>36895</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>43</v>
@@ -571,13 +571,13 @@
         <v>36896</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>63</v>
@@ -595,13 +595,13 @@
         <v>36897</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7">
         <v>53</v>
@@ -619,13 +619,13 @@
         <v>36897</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>53</v>
@@ -643,13 +643,13 @@
         <v>36899</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E9">
         <v>86</v>
@@ -667,13 +667,13 @@
         <v>36900</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10">
         <v>54</v>
@@ -691,13 +691,13 @@
         <v>36901</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E11">
         <v>65</v>
@@ -715,13 +715,13 @@
         <v>36902</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12">
         <v>42</v>
@@ -739,13 +739,13 @@
         <v>36903</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>43</v>
@@ -763,13 +763,13 @@
         <v>36904</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14">
         <v>109</v>
@@ -787,13 +787,13 @@
         <v>36905</v>
       </c>
       <c r="B15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15">
         <v>24</v>
@@ -811,13 +811,13 @@
         <v>36905</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E16">
         <v>53</v>
@@ -835,13 +835,13 @@
         <v>36907</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17">
         <v>64</v>

</xml_diff>